<commit_message>
Change permCAF label to proCAF
</commit_message>
<xml_diff>
--- a/results/tables/UNC-bulk_clinical_and_molecular_data.xlsx
+++ b/results/tables/UNC-bulk_clinical_and_molecular_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t xml:space="preserve">sampID</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permCAF</t>
   </si>
   <si>
     <t xml:space="preserve">Strong permCAF</t>
@@ -981,20 +978,18 @@
       <c r="G3" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3"/>
+      <c r="I3" t="s">
         <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
       </c>
       <c r="J3" t="n">
         <v>0.991222759649319</v>
       </c>
       <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
         <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
       </c>
       <c r="M3" t="n">
         <v>1</v>
@@ -1008,7 +1003,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="n">
         <v>25.3963039014374</v>
@@ -1055,7 +1050,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="n">
         <v>146.464065708419</v>
@@ -1064,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1102,7 +1097,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="n">
         <v>10.1848049281314</v>
@@ -1114,7 +1109,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
@@ -1126,7 +1121,7 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" t="n">
         <v>0.00109570513676018</v>
@@ -1149,7 +1144,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="n">
         <v>1.1170431211499</v>
@@ -1196,7 +1191,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="n">
         <v>19.4496919917864</v>
@@ -1243,7 +1238,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="n">
         <v>32.3613963039014</v>
@@ -1255,7 +1250,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
         <v>18</v>
@@ -1263,11 +1258,9 @@
       <c r="G9" t="n">
         <v>0.947524078172082</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9"/>
+      <c r="I9" t="s">
         <v>26</v>
-      </c>
-      <c r="I9" t="s">
-        <v>27</v>
       </c>
       <c r="J9" t="n">
         <v>0.00276888224790701</v>
@@ -1290,7 +1283,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="n">
         <v>12.8788501026694</v>
@@ -1314,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" t="n">
         <v>0.00449125584309229</v>
@@ -1337,7 +1330,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="n">
         <v>17.741273100616</v>
@@ -1357,11 +1350,9 @@
       <c r="G11" t="n">
         <v>0.947524078172082</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11"/>
+      <c r="I11" t="s">
         <v>26</v>
-      </c>
-      <c r="I11" t="s">
-        <v>27</v>
       </c>
       <c r="J11" t="n">
         <v>0.0768595570582297</v>
@@ -1384,7 +1375,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="n">
         <v>7.19507186858316</v>
@@ -1404,11 +1395,9 @@
       <c r="G12" t="n">
         <v>0.998826874466896</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12"/>
+      <c r="I12" t="s">
         <v>26</v>
-      </c>
-      <c r="I12" t="s">
-        <v>27</v>
       </c>
       <c r="J12" t="n">
         <v>0.00109570513676018</v>
@@ -1431,7 +1420,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" t="n">
         <v>9.13347022587269</v>
@@ -1478,7 +1467,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="n">
         <v>18.7926078028747</v>
@@ -1490,7 +1479,7 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -1525,7 +1514,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="n">
         <v>101.782340862423</v>
@@ -1572,7 +1561,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="n">
         <v>18.5954825462012</v>
@@ -1602,10 +1591,10 @@
         <v>0.646673207899976</v>
       </c>
       <c r="K16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
@@ -1619,7 +1608,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="n">
         <v>8.80492813141684</v>
@@ -1631,7 +1620,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
         <v>18</v>
@@ -1666,7 +1655,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" t="n">
         <v>11.6960985626283</v>
@@ -1686,11 +1675,9 @@
       <c r="G18" t="n">
         <v>0.778495610458788</v>
       </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
+      <c r="H18"/>
       <c r="I18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J18" t="n">
         <v>0.0069303512042848</v>
@@ -1713,7 +1700,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="n">
         <v>4.76386036960986</v>
@@ -1733,11 +1720,9 @@
       <c r="G19" t="n">
         <v>0.947524078172082</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19"/>
+      <c r="I19" t="s">
         <v>26</v>
-      </c>
-      <c r="I19" t="s">
-        <v>27</v>
       </c>
       <c r="J19" t="n">
         <v>0.00109570513676018</v>
@@ -1760,7 +1745,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="n">
         <v>44.1232032854209</v>
@@ -1780,11 +1765,9 @@
       <c r="G20" t="n">
         <v>0.972185984054384</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20"/>
+      <c r="I20" t="s">
         <v>26</v>
-      </c>
-      <c r="I20" t="s">
-        <v>27</v>
       </c>
       <c r="J20" t="n">
         <v>0.0505131198470057</v>
@@ -1807,7 +1790,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" t="n">
         <v>1.01848049281314</v>
@@ -1827,20 +1810,18 @@
       <c r="G21" t="n">
         <v>0.94443220152151</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21"/>
+      <c r="I21" t="s">
         <v>26</v>
-      </c>
-      <c r="I21" t="s">
-        <v>27</v>
       </c>
       <c r="J21" t="n">
         <v>0.904450962740972</v>
       </c>
       <c r="K21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" t="s">
         <v>28</v>
-      </c>
-      <c r="L21" t="s">
-        <v>29</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -1854,7 +1835,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="n">
         <v>25.7248459958932</v>
@@ -1901,7 +1882,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" t="n">
         <v>72.9034907597536</v>
@@ -1942,7 +1923,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="n">
         <v>14.1273100616016</v>
@@ -1954,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
         <v>18</v>
@@ -1989,7 +1970,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" t="n">
         <v>10.4147843942505</v>
@@ -2009,11 +1990,9 @@
       <c r="G25" t="n">
         <v>0.94443220152151</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25"/>
+      <c r="I25" t="s">
         <v>26</v>
-      </c>
-      <c r="I25" t="s">
-        <v>27</v>
       </c>
       <c r="J25" t="n">
         <v>0.00549982125042632</v>
@@ -2036,7 +2015,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" t="n">
         <v>1.51129363449692</v>
@@ -2077,7 +2056,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" t="n">
         <v>31.605749486653</v>
@@ -2089,7 +2068,7 @@
         <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
         <v>18</v>
@@ -2124,7 +2103,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" t="n">
         <v>21.6509240246407</v>
@@ -2171,7 +2150,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" t="n">
         <v>51.8110882956879</v>
@@ -2191,11 +2170,9 @@
       <c r="G29" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29"/>
+      <c r="I29" t="s">
         <v>26</v>
-      </c>
-      <c r="I29" t="s">
-        <v>27</v>
       </c>
       <c r="J29" t="n">
         <v>0.0129174813257915</v>
@@ -2218,7 +2195,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" t="n">
         <v>7.45790554414784</v>
@@ -2265,7 +2242,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" t="n">
         <v>14.2915811088296</v>
@@ -2312,7 +2289,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" t="n">
         <v>40.6078028747433</v>
@@ -2324,7 +2301,7 @@
         <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
         <v>18</v>
@@ -2336,7 +2313,7 @@
         <v>19</v>
       </c>
       <c r="I32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J32" t="n">
         <v>0.0112122472072454</v>
@@ -2359,7 +2336,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" t="n">
         <v>15.8685831622177</v>
@@ -2377,11 +2354,9 @@
       <c r="G33" t="n">
         <v>0.630856721870069</v>
       </c>
-      <c r="H33" t="s">
-        <v>26</v>
-      </c>
+      <c r="H33"/>
       <c r="I33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J33" t="n">
         <v>0.00276888224790701</v>
@@ -2404,7 +2379,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" t="n">
         <v>14.2258726899384</v>
@@ -2449,7 +2424,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" t="n">
         <v>29.9958932238193</v>
@@ -2469,11 +2444,9 @@
       <c r="G35" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35"/>
+      <c r="I35" t="s">
         <v>26</v>
-      </c>
-      <c r="I35" t="s">
-        <v>27</v>
       </c>
       <c r="J35" t="n">
         <v>0.0907121498422687</v>
@@ -2496,7 +2469,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" t="n">
         <v>63.6386036960986</v>
@@ -2508,7 +2481,7 @@
         <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
         <v>18</v>
@@ -2543,7 +2516,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" t="n">
         <v>61.2731006160164</v>
@@ -2584,7 +2557,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" t="n">
         <v>55.2607802874743</v>
@@ -2608,7 +2581,7 @@
         <v>19</v>
       </c>
       <c r="I38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J38" t="n">
         <v>0.00109570513676018</v>
@@ -2625,7 +2598,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" t="n">
         <v>21.7166324435318</v>
@@ -2672,7 +2645,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" t="n">
         <v>20.6652977412731</v>
@@ -2713,7 +2686,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" t="n">
         <v>27.1375770020534</v>
@@ -2760,7 +2733,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" t="n">
         <v>17.6755646817248</v>
@@ -2784,16 +2757,16 @@
         <v>19</v>
       </c>
       <c r="I42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J42" t="n">
         <v>0.902224016368246</v>
       </c>
       <c r="K42" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" t="s">
         <v>28</v>
-      </c>
-      <c r="L42" t="s">
-        <v>29</v>
       </c>
       <c r="M42"/>
       <c r="N42"/>
@@ -2801,7 +2774,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" t="n">
         <v>6.57084188911704</v>
@@ -2848,7 +2821,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" t="n">
         <v>12.8131416837782</v>
@@ -2895,7 +2868,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" t="n">
         <v>16.5256673511294</v>
@@ -2907,7 +2880,7 @@
         <v>16</v>
       </c>
       <c r="E45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F45" t="s">
         <v>18</v>
@@ -2919,7 +2892,7 @@
         <v>19</v>
       </c>
       <c r="I45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J45" t="n">
         <v>0.199531707115296</v>
@@ -2928,7 +2901,7 @@
         <v>21</v>
       </c>
       <c r="L45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M45"/>
       <c r="N45"/>
@@ -2936,7 +2909,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B46" t="n">
         <v>44.7145790554415</v>
@@ -2975,7 +2948,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" t="n">
         <v>43.8275154004107</v>
@@ -2987,7 +2960,7 @@
         <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F47" t="s">
         <v>18</v>
@@ -3016,7 +2989,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" t="n">
         <v>13.7330595482546</v>
@@ -3036,11 +3009,9 @@
       <c r="G48" t="n">
         <v>0.778495610458788</v>
       </c>
-      <c r="H48" t="s">
-        <v>26</v>
-      </c>
+      <c r="H48"/>
       <c r="I48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J48" t="n">
         <v>0.00109570513676018</v>
@@ -3063,7 +3034,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" t="n">
         <v>9.62628336755647</v>
@@ -3083,11 +3054,9 @@
       <c r="G49" t="n">
         <v>0.630856721870069</v>
       </c>
-      <c r="H49" t="s">
-        <v>26</v>
-      </c>
+      <c r="H49"/>
       <c r="I49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J49" t="n">
         <v>0.00109570513676018</v>
@@ -3110,7 +3079,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" t="n">
         <v>35.482546201232</v>
@@ -3157,7 +3126,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" t="n">
         <v>12.7474332648871</v>
@@ -3169,7 +3138,7 @@
         <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F51" t="s">
         <v>18</v>
@@ -3187,10 +3156,10 @@
         <v>0.957264143793731</v>
       </c>
       <c r="K51" t="s">
+        <v>27</v>
+      </c>
+      <c r="L51" t="s">
         <v>28</v>
-      </c>
-      <c r="L51" t="s">
-        <v>29</v>
       </c>
       <c r="M51"/>
       <c r="N51"/>
@@ -3198,7 +3167,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" t="n">
         <v>34.9897330595483</v>
@@ -3210,7 +3179,7 @@
         <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F52" t="s">
         <v>18</v>
@@ -3245,7 +3214,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" t="n">
         <v>16.2628336755647</v>
@@ -3292,7 +3261,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" t="n">
         <v>5.02669404517454</v>
@@ -3322,10 +3291,10 @@
         <v>0.646673207899976</v>
       </c>
       <c r="K54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M54" t="n">
         <v>1</v>
@@ -3339,7 +3308,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B55" t="n">
         <v>10.3490759753593</v>
@@ -3384,7 +3353,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" t="n">
         <v>16.0657084188912</v>
@@ -3404,11 +3373,9 @@
       <c r="G56" t="n">
         <v>0.630856721870069</v>
       </c>
-      <c r="H56" t="s">
-        <v>26</v>
-      </c>
+      <c r="H56"/>
       <c r="I56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J56" t="n">
         <v>0.0332488851287233</v>
@@ -3431,7 +3398,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B57" t="n">
         <v>10.217659137577</v>
@@ -3478,7 +3445,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" t="n">
         <v>12.8131416837782</v>
@@ -3519,7 +3486,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B59" t="n">
         <v>7.09650924024641</v>
@@ -3539,11 +3506,9 @@
       <c r="G59" t="n">
         <v>0.778495610458788</v>
       </c>
-      <c r="H59" t="s">
-        <v>26</v>
-      </c>
+      <c r="H59"/>
       <c r="I59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J59" t="n">
         <v>0.00276888224790701</v>
@@ -3566,7 +3531,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" t="n">
         <v>0.624229979466119</v>
@@ -3613,7 +3578,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B61" t="n">
         <v>8.18069815195072</v>
@@ -3625,7 +3590,7 @@
         <v>16</v>
       </c>
       <c r="E61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F61" t="s">
         <v>18</v>
@@ -3660,7 +3625,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B62" t="n">
         <v>19.9096509240246</v>
@@ -3707,7 +3672,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B63" t="n">
         <v>19.3511293634497</v>
@@ -3727,11 +3692,9 @@
       <c r="G63" t="n">
         <v>0.94087326957571</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63"/>
+      <c r="I63" t="s">
         <v>26</v>
-      </c>
-      <c r="I63" t="s">
-        <v>27</v>
       </c>
       <c r="J63" t="n">
         <v>0.00109570513676018</v>
@@ -3754,7 +3717,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B64" t="n">
         <v>19.1868583162218</v>
@@ -3801,7 +3764,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B65" t="n">
         <v>1.08418891170431</v>
@@ -3819,11 +3782,9 @@
       <c r="G65" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65"/>
+      <c r="I65" t="s">
         <v>26</v>
-      </c>
-      <c r="I65" t="s">
-        <v>27</v>
       </c>
       <c r="J65" t="n">
         <v>0.00177914157667774</v>
@@ -3846,7 +3807,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B66" t="n">
         <v>7.12936344969199</v>
@@ -3866,11 +3827,9 @@
       <c r="G66" t="n">
         <v>0.947524078172082</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66"/>
+      <c r="I66" t="s">
         <v>26</v>
-      </c>
-      <c r="I66" t="s">
-        <v>27</v>
       </c>
       <c r="J66" t="n">
         <v>0.0926075227236015</v>
@@ -3887,7 +3846,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B67" t="n">
         <v>26.2505133470226</v>
@@ -3934,7 +3893,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B68" t="n">
         <v>3.58110882956879</v>
@@ -3975,7 +3934,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B69" t="n">
         <v>5.02669404517454</v>
@@ -4016,7 +3975,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B70" t="n">
         <v>129.215605749487</v>
@@ -4057,7 +4016,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B71" t="n">
         <v>7.65503080082136</v>
@@ -4104,7 +4063,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B72" t="n">
         <v>43.7946611909651</v>
@@ -4124,11 +4083,9 @@
       <c r="G72" t="n">
         <v>0.630856721870069</v>
       </c>
-      <c r="H72" t="s">
-        <v>26</v>
-      </c>
+      <c r="H72"/>
       <c r="I72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J72" t="n">
         <v>0.00449125584309229</v>
@@ -4151,7 +4108,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B73" t="n">
         <v>12.0903490759754</v>
@@ -4171,11 +4128,9 @@
       <c r="G73" t="n">
         <v>0.911674039831992</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H73"/>
+      <c r="I73" t="s">
         <v>26</v>
-      </c>
-      <c r="I73" t="s">
-        <v>27</v>
       </c>
       <c r="J73" t="n">
         <v>0.0069303512042848</v>
@@ -4198,7 +4153,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B74" t="n">
         <v>56.5749486652977</v>
@@ -4245,7 +4200,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B75" t="n">
         <v>80.5913757700205</v>
@@ -4292,7 +4247,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B76" t="n">
         <v>19.0225872689938</v>
@@ -4333,7 +4288,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B77" t="n">
         <v>0.75564681724846</v>
@@ -4357,7 +4312,7 @@
         <v>19</v>
       </c>
       <c r="I77" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J77" t="n">
         <v>0.00109570513676018</v>
@@ -4380,7 +4335,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B78" t="n">
         <v>50.135523613963</v>
@@ -4427,7 +4382,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B79" t="n">
         <v>13.2073921971253</v>
@@ -4474,7 +4429,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B80" t="n">
         <v>3.5482546201232</v>
@@ -4486,7 +4441,7 @@
         <v>16</v>
       </c>
       <c r="E80" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F80" t="s">
         <v>18</v>
@@ -4521,7 +4476,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B81" t="n">
         <v>19.6139630390144</v>
@@ -4545,7 +4500,7 @@
         <v>19</v>
       </c>
       <c r="I81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J81" t="n">
         <v>0.00276888224790701</v>
@@ -4568,7 +4523,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B82" t="n">
         <v>14.258726899384</v>
@@ -4580,7 +4535,7 @@
         <v>16</v>
       </c>
       <c r="E82" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F82" t="s">
         <v>18</v>
@@ -4615,7 +4570,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B83" t="n">
         <v>45.1416837782341</v>
@@ -4662,7 +4617,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B84" t="n">
         <v>10.4147843942505</v>
@@ -4709,7 +4664,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B85" t="n">
         <v>102.99794661191</v>
@@ -4756,7 +4711,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B86" t="n">
         <v>10.0205338809035</v>
@@ -4786,10 +4741,10 @@
         <v>0.55688079984102</v>
       </c>
       <c r="K86" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M86" t="n">
         <v>1</v>
@@ -4803,7 +4758,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B87" t="n">
         <v>2.36550308008214</v>
@@ -4844,7 +4799,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B88" t="n">
         <v>8.77207392197125</v>
@@ -4868,7 +4823,7 @@
         <v>19</v>
       </c>
       <c r="I88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J88" t="n">
         <v>0.00109570513676018</v>
@@ -4891,7 +4846,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B89" t="n">
         <v>8.2135523613963</v>
@@ -4915,7 +4870,7 @@
         <v>19</v>
       </c>
       <c r="I89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J89" t="n">
         <v>0.00794298615675521</v>
@@ -4938,7 +4893,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B90" t="n">
         <v>39.0308008213552</v>
@@ -4979,7 +4934,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B91" t="n">
         <v>5.97946611909651</v>
@@ -4999,20 +4954,18 @@
       <c r="G91" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91"/>
+      <c r="I91" t="s">
         <v>26</v>
-      </c>
-      <c r="I91" t="s">
-        <v>27</v>
       </c>
       <c r="J91" t="n">
         <v>0.902224016368246</v>
       </c>
       <c r="K91" t="s">
+        <v>27</v>
+      </c>
+      <c r="L91" t="s">
         <v>28</v>
-      </c>
-      <c r="L91" t="s">
-        <v>29</v>
       </c>
       <c r="M91" t="n">
         <v>1</v>
@@ -5026,7 +4979,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B92" t="n">
         <v>18.8583162217659</v>
@@ -5073,7 +5026,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B93" t="n">
         <v>4.96098562628337</v>
@@ -5085,7 +5038,7 @@
         <v>24</v>
       </c>
       <c r="E93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F93" t="s">
         <v>18</v>
@@ -5093,11 +5046,9 @@
       <c r="G93" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H93"/>
+      <c r="I93" t="s">
         <v>26</v>
-      </c>
-      <c r="I93" t="s">
-        <v>27</v>
       </c>
       <c r="J93" t="n">
         <v>0.38826766626129</v>
@@ -5106,7 +5057,7 @@
         <v>21</v>
       </c>
       <c r="L93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M93" t="n">
         <v>1</v>
@@ -5120,7 +5071,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B94" t="n">
         <v>20.6324435318275</v>
@@ -5167,7 +5118,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B95" t="n">
         <v>1.74127310061602</v>
@@ -5197,10 +5148,10 @@
         <v>0.859537904815494</v>
       </c>
       <c r="K95" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L95" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M95" t="n">
         <v>0</v>
@@ -5214,7 +5165,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B96" t="n">
         <v>11.4661190965092</v>
@@ -5261,7 +5212,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B97" t="n">
         <v>17.0513347022587</v>
@@ -5308,7 +5259,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B98" t="n">
         <v>21.5523613963039</v>
@@ -5320,7 +5271,7 @@
         <v>16</v>
       </c>
       <c r="E98" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F98" t="s">
         <v>18</v>
@@ -5355,7 +5306,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B99" t="n">
         <v>99.3839835728953</v>
@@ -5402,7 +5353,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B100" t="n">
         <v>8.27926078028747</v>
@@ -5414,7 +5365,7 @@
         <v>16</v>
       </c>
       <c r="E100" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F100" t="s">
         <v>18</v>
@@ -5449,7 +5400,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B101" t="n">
         <v>9.79055441478439</v>
@@ -5496,7 +5447,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B102" t="n">
         <v>11.5318275154004</v>
@@ -5516,11 +5467,9 @@
       <c r="G102" t="n">
         <v>0.509289514032634</v>
       </c>
-      <c r="H102" t="s">
-        <v>26</v>
-      </c>
+      <c r="H102"/>
       <c r="I102" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J102" t="n">
         <v>0.0330222682372176</v>
@@ -5543,7 +5492,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B103" t="n">
         <v>93.7330595482546</v>
@@ -5590,7 +5539,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B104" t="n">
         <v>25.429158110883</v>
@@ -5614,7 +5563,7 @@
         <v>19</v>
       </c>
       <c r="I104" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J104" t="n">
         <v>0.00109570513676018</v>
@@ -5637,7 +5586,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B105" t="n">
         <v>30.0616016427105</v>
@@ -5684,7 +5633,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B106" t="n">
         <v>81.4784394250513</v>
@@ -5731,7 +5680,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B107" t="n">
         <v>4.92813141683778</v>
@@ -5751,20 +5700,18 @@
       <c r="G107" t="n">
         <v>0.998826874466896</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H107"/>
+      <c r="I107" t="s">
         <v>26</v>
-      </c>
-      <c r="I107" t="s">
-        <v>27</v>
       </c>
       <c r="J107" t="n">
         <v>0.671478445024693</v>
       </c>
       <c r="K107" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L107" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M107" t="n">
         <v>1</v>
@@ -5778,7 +5725,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B108" t="n">
         <v>123.696098562628</v>
@@ -5790,7 +5737,7 @@
         <v>16</v>
       </c>
       <c r="E108" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F108" t="s">
         <v>18</v>
@@ -5802,7 +5749,7 @@
         <v>19</v>
       </c>
       <c r="I108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J108" t="n">
         <v>0.00449125584309229</v>
@@ -5825,7 +5772,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B109" t="n">
         <v>0.0657084188911704</v>
@@ -5845,20 +5792,18 @@
       <c r="G109" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H109" t="s">
+      <c r="H109"/>
+      <c r="I109" t="s">
         <v>26</v>
-      </c>
-      <c r="I109" t="s">
-        <v>27</v>
       </c>
       <c r="J109" t="n">
         <v>0.991222759649319</v>
       </c>
       <c r="K109" t="s">
+        <v>27</v>
+      </c>
+      <c r="L109" t="s">
         <v>28</v>
-      </c>
-      <c r="L109" t="s">
-        <v>29</v>
       </c>
       <c r="M109"/>
       <c r="N109"/>
@@ -5866,7 +5811,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B110" t="n">
         <v>4.23819301848049</v>
@@ -5886,20 +5831,18 @@
       <c r="G110" t="n">
         <v>0.833858157810455</v>
       </c>
-      <c r="H110" t="s">
-        <v>26</v>
-      </c>
+      <c r="H110"/>
       <c r="I110" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J110" t="n">
         <v>0.991222759649319</v>
       </c>
       <c r="K110" t="s">
+        <v>27</v>
+      </c>
+      <c r="L110" t="s">
         <v>28</v>
-      </c>
-      <c r="L110" t="s">
-        <v>29</v>
       </c>
       <c r="M110" t="n">
         <v>1</v>
@@ -5913,7 +5856,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B111" t="n">
         <v>25.7905544147844</v>
@@ -5933,11 +5876,9 @@
       <c r="G111" t="n">
         <v>0.767884290338677</v>
       </c>
-      <c r="H111" t="s">
-        <v>26</v>
-      </c>
+      <c r="H111"/>
       <c r="I111" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J111" t="n">
         <v>0.00109570513676018</v>
@@ -5960,7 +5901,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B112" t="n">
         <v>54.8665297741273</v>
@@ -6007,7 +5948,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B113" t="n">
         <v>18.3655030800821</v>
@@ -6027,11 +5968,9 @@
       <c r="G113" t="n">
         <v>0.998826874466896</v>
       </c>
-      <c r="H113" t="s">
+      <c r="H113"/>
+      <c r="I113" t="s">
         <v>26</v>
-      </c>
-      <c r="I113" t="s">
-        <v>27</v>
       </c>
       <c r="J113" t="n">
         <v>0.28089687800887</v>
@@ -6040,7 +5979,7 @@
         <v>21</v>
       </c>
       <c r="L113" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M113" t="n">
         <v>1</v>
@@ -6054,7 +5993,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B114" t="n">
         <v>22.0780287474333</v>
@@ -6101,7 +6040,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B115" t="n">
         <v>48.3285420944559</v>
@@ -6148,7 +6087,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B116" t="n">
         <v>47.4414784394251</v>
@@ -6195,7 +6134,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B117" t="n">
         <v>16.8542094455852</v>
@@ -6207,7 +6146,7 @@
         <v>16</v>
       </c>
       <c r="E117" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F117" t="s">
         <v>18</v>
@@ -6242,7 +6181,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B118" t="n">
         <v>43.1375770020534</v>
@@ -6289,7 +6228,7 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B119" t="n">
         <v>21.4537987679671</v>
@@ -6336,7 +6275,7 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B120" t="n">
         <v>7.39219712525667</v>
@@ -6356,11 +6295,9 @@
       <c r="G120" t="n">
         <v>0.767884290338677</v>
       </c>
-      <c r="H120" t="s">
-        <v>26</v>
-      </c>
+      <c r="H120"/>
       <c r="I120" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J120" t="n">
         <v>0.00109570513676018</v>
@@ -6383,7 +6320,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B121" t="n">
         <v>27.564681724846</v>
@@ -6430,7 +6367,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B122" t="n">
         <v>5.88090349075975</v>
@@ -6450,11 +6387,9 @@
       <c r="G122" t="n">
         <v>0.996038453037659</v>
       </c>
-      <c r="H122" t="s">
+      <c r="H122"/>
+      <c r="I122" t="s">
         <v>26</v>
-      </c>
-      <c r="I122" t="s">
-        <v>27</v>
       </c>
       <c r="J122" t="n">
         <v>0.0138052803325107</v>
@@ -6471,7 +6406,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B123" t="n">
         <v>8.47638603696099</v>
@@ -6512,7 +6447,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B124" t="n">
         <v>8.18069815195072</v>
@@ -6559,7 +6494,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B125" t="n">
         <v>6.83367556468172</v>
@@ -6579,11 +6514,9 @@
       <c r="G125" t="n">
         <v>0.972185984054384</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H125"/>
+      <c r="I125" t="s">
         <v>26</v>
-      </c>
-      <c r="I125" t="s">
-        <v>27</v>
       </c>
       <c r="J125" t="n">
         <v>0.00109570513676018</v>
@@ -6606,7 +6539,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B126" t="n">
         <v>28.3203285420945</v>
@@ -6647,7 +6580,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B127" t="n">
         <v>11.4004106776181</v>
@@ -6667,20 +6600,18 @@
       <c r="G127" t="n">
         <v>0.981491175780394</v>
       </c>
-      <c r="H127" t="s">
+      <c r="H127"/>
+      <c r="I127" t="s">
         <v>26</v>
-      </c>
-      <c r="I127" t="s">
-        <v>27</v>
       </c>
       <c r="J127" t="n">
         <v>0.991222759649319</v>
       </c>
       <c r="K127" t="s">
+        <v>27</v>
+      </c>
+      <c r="L127" t="s">
         <v>28</v>
-      </c>
-      <c r="L127" t="s">
-        <v>29</v>
       </c>
       <c r="M127" t="n">
         <v>1</v>
@@ -6694,7 +6625,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B128" t="n">
         <v>15.1129363449692</v>
@@ -6714,11 +6645,9 @@
       <c r="G128" t="n">
         <v>0.994462085754022</v>
       </c>
-      <c r="H128" t="s">
+      <c r="H128"/>
+      <c r="I128" t="s">
         <v>26</v>
-      </c>
-      <c r="I128" t="s">
-        <v>27</v>
       </c>
       <c r="J128" t="n">
         <v>0.00276888224790701</v>
@@ -6741,7 +6670,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B129" t="n">
         <v>17.6755646817248</v>
@@ -6782,7 +6711,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B130" t="n">
         <v>2.75975359342916</v>
@@ -6794,7 +6723,7 @@
         <v>16</v>
       </c>
       <c r="E130" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F130" t="s">
         <v>18</v>
@@ -6802,11 +6731,9 @@
       <c r="G130" t="n">
         <v>0.767884290338678</v>
       </c>
-      <c r="H130" t="s">
-        <v>26</v>
-      </c>
+      <c r="H130"/>
       <c r="I130" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J130" t="n">
         <v>0.00109570513676018</v>

</xml_diff>